<commit_message>
Comparis taxass interactive plot
</commit_message>
<xml_diff>
--- a/Figures/Paper/Comparison-Taxonomy/Compare.xlsx
+++ b/Figures/Paper/Comparison-Taxonomy/Compare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patriciatran/Documents/Github/LakeTanganyika/Figures/Paper/Comparison-Taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BCA3C347-F0C9-A44F-B0A0-FAEE64DFD8C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A137BDA6-B6E1-364E-B7DB-E22620EB224D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" xr2:uid="{3DFF2FF1-021C-514F-B705-EFA909E61CB9}"/>
   </bookViews>
@@ -3219,10 +3219,10 @@
     <t>Yes but Deltaproteobacteria are Myxococcota</t>
   </si>
   <si>
-    <t>Sericytochromatia Tanganyikabacteria</t>
-  </si>
-  <si>
     <t>Yes for RP16 and GTDB but could not get the same resolution with TaxAss</t>
+  </si>
+  <si>
+    <t>Sericytochromatia, Tanganyikabacteria</t>
   </si>
 </sst>
 </file>
@@ -3366,17 +3366,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3699,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61670AF6-77EA-0848-B75C-B089BA3E4D34}">
   <dimension ref="A1:M525"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C183" workbookViewId="0">
-      <selection activeCell="G185" sqref="G185"/>
+    <sheetView tabSelected="1" topLeftCell="A481" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D496" sqref="D496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7997,7 +7987,7 @@
         <v>891</v>
       </c>
       <c r="G202" s="15" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
@@ -10280,7 +10270,7 @@
         <v>935</v>
       </c>
       <c r="G307" s="15" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.2">
@@ -14245,7 +14235,7 @@
         <v>7.58</v>
       </c>
       <c r="D493" s="1" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="E493" s="3" t="s">
         <v>692</v>
@@ -14264,7 +14254,7 @@
         <v>0.85</v>
       </c>
       <c r="D494" s="1" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="E494" s="3" t="s">
         <v>692</v>
@@ -14287,7 +14277,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="D495" s="1" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="E495" s="3" t="s">
         <v>693</v>
@@ -14942,6 +14932,7 @@
       <c r="F525" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G525" xr:uid="{8D0E96A6-D640-1844-9AF0-6B62BEC8F6FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M524">
     <sortCondition ref="D2:D524"/>
   </sortState>

</xml_diff>